<commit_message>
Fix data and logic
</commit_message>
<xml_diff>
--- a/docs/numbers_type.xlsx
+++ b/docs/numbers_type.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\at4\MPLABXProjects\random_number_oled.X\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\at4\MPLABXProjects\random_numbers_OLED.X\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5678DC-D171-4FD8-8067-AF792080224E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEF34D4-C063-4527-AC82-5DDC9678B36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="735" windowWidth="25590" windowHeight="20490" xr2:uid="{62E818D9-7243-4E8C-AE33-69A5B8F80369}"/>
+    <workbookView xWindow="1680" yWindow="660" windowWidth="25590" windowHeight="20490" xr2:uid="{62E818D9-7243-4E8C-AE33-69A5B8F80369}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -548,7 +548,7 @@
   <dimension ref="A1:CR49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.375" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -645,7 +645,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
@@ -684,7 +684,7 @@
       <c r="AT2" s="7"/>
       <c r="AU2" s="6"/>
       <c r="AV2" s="8"/>
-      <c r="AW2" s="9"/>
+      <c r="AW2" s="15"/>
       <c r="AX2" s="7"/>
       <c r="AY2" s="7"/>
       <c r="AZ2" s="7"/>
@@ -726,7 +726,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="I3" s="6"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
@@ -766,7 +766,7 @@
       <c r="AT3" s="7"/>
       <c r="AU3" s="6"/>
       <c r="AV3" s="8"/>
-      <c r="AW3" s="9"/>
+      <c r="AW3" s="15"/>
       <c r="AX3" s="7"/>
       <c r="AY3" s="7"/>
       <c r="AZ3" s="7"/>
@@ -807,7 +807,7 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
@@ -888,7 +888,7 @@
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
@@ -930,7 +930,7 @@
       <c r="AT5" s="7"/>
       <c r="AU5" s="7"/>
       <c r="AV5" s="8"/>
-      <c r="AW5" s="9"/>
+      <c r="AW5" s="15"/>
       <c r="AX5" s="7"/>
       <c r="AY5" s="7"/>
       <c r="AZ5" s="7"/>
@@ -969,7 +969,7 @@
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -1012,7 +1012,7 @@
       <c r="AT6" s="7"/>
       <c r="AU6" s="7"/>
       <c r="AV6" s="8"/>
-      <c r="AW6" s="9"/>
+      <c r="AW6" s="15"/>
       <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
       <c r="AZ6" s="7"/>
@@ -1028,7 +1028,7 @@
       <c r="BJ6" s="7"/>
       <c r="BK6" s="6"/>
       <c r="BL6" s="8"/>
-      <c r="BM6" s="9"/>
+      <c r="BM6" s="15"/>
       <c r="BN6" s="7"/>
       <c r="BO6" s="7"/>
       <c r="BP6" s="7"/>
@@ -1110,7 +1110,7 @@
       <c r="BJ7" s="6"/>
       <c r="BK7" s="6"/>
       <c r="BL7" s="8"/>
-      <c r="BM7" s="9"/>
+      <c r="BM7" s="15"/>
       <c r="BN7" s="7"/>
       <c r="BO7" s="7"/>
       <c r="BP7" s="7"/>
@@ -1666,7 +1666,7 @@
       <c r="BJ13" s="16"/>
       <c r="BK13" s="6"/>
       <c r="BL13" s="8"/>
-      <c r="BM13" s="9"/>
+      <c r="BM13" s="15"/>
       <c r="BN13" s="7"/>
       <c r="BO13" s="7"/>
       <c r="BP13" s="7"/>
@@ -1764,7 +1764,7 @@
       <c r="BJ14" s="16"/>
       <c r="BK14" s="6"/>
       <c r="BL14" s="8"/>
-      <c r="BM14" s="9"/>
+      <c r="BM14" s="15"/>
       <c r="BN14" s="7"/>
       <c r="BO14" s="7"/>
       <c r="BP14" s="7"/>

</xml_diff>